<commit_message>
pibix última versão e dataset termosporconcelho sem açores
</commit_message>
<xml_diff>
--- a/Arquivos/Dataset/termos_Concelho.xlsx
+++ b/Arquivos/Dataset/termos_Concelho.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto PP\GymTrend-Task-Force\Arquivos\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\Projectos\UPskill\Projecto Power\GymTrend-Task-Force\Arquivos\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA793FA-DAC6-4277-A78F-F66DEA941593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29EABF6-70B1-4392-844B-D59F9D923D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E34A085-28B9-4C2F-B6B4-95072BA85716}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E34A085-28B9-4C2F-B6B4-95072BA85716}"/>
   </bookViews>
   <sheets>
     <sheet name="geoMap_ginasios" sheetId="2" r:id="rId1"/>
     <sheet name="Folha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">geoMap_ginasios!$A$1:$C$385</definedName>
+    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">geoMap_ginasios!$A$1:$C$377</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="101">
   <si>
     <t>Cidade</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Ovar</t>
   </si>
   <si>
-    <t>Ponta Delgada</t>
-  </si>
-  <si>
     <t>Torres Vedras</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
   </si>
   <si>
     <t>Castro Marim</t>
-  </si>
-  <si>
-    <t>Ponta do Sol</t>
   </si>
   <si>
     <t>Cinfães</t>
@@ -430,9 +424,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A195936-3802-4C35-B43F-EA489C118242}" name="geoMap_ginasios" displayName="geoMap_ginasios" ref="A1:C385" tableType="queryTable" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C385">
-    <sortCondition descending="1" ref="C1:C385"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A195936-3802-4C35-B43F-EA489C118242}" name="geoMap_ginasios" displayName="geoMap_ginasios" ref="A1:C377" tableType="queryTable" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C377">
+    <sortCondition descending="1" ref="C1:C377"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A9E2DA8B-F642-49DB-ADE4-156FEEA4D67D}" uniqueName="1" name="Cidade" queryTableFieldId="1" dataDxfId="1"/>
@@ -740,11 +734,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC44209-7355-4A65-9607-267A54FB324D}">
-  <dimension ref="A1:C385"/>
+  <dimension ref="A1:C377"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -769,7 +761,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -780,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -791,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -802,7 +794,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -813,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -824,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -835,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -846,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -857,7 +849,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -868,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -879,7 +871,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -890,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -901,10 +893,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -912,10 +904,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -923,7 +915,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16">
         <v>0.75</v>
@@ -934,10 +926,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17">
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -945,10 +937,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18">
-        <v>0.73</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -956,10 +948,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19">
-        <v>0.69</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -967,51 +959,51 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20">
-        <v>0.67</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21">
-        <v>0.57999999999999996</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22">
-        <v>0.28999999999999998</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24">
         <v>0.22</v>
@@ -1022,7 +1014,7 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25">
         <v>0.22</v>
@@ -1030,10 +1022,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C26">
         <v>0.22</v>
@@ -1041,32 +1033,32 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29">
         <v>0.16</v>
@@ -1074,54 +1066,54 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C33">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C34">
         <v>0.06</v>
@@ -1129,54 +1121,54 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1198,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1206,10 +1198,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1231,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1239,10 +1231,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1264,7 +1256,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1272,10 +1264,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1297,7 +1289,7 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1305,10 +1297,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1316,10 +1308,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1341,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1349,10 +1341,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1374,7 +1366,7 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1382,10 +1374,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1407,7 +1399,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1415,10 +1407,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1440,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1448,10 +1440,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1473,7 +1465,7 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1481,10 +1473,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1506,7 +1498,7 @@
         <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1514,10 +1506,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1536,10 +1528,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1547,10 +1539,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1558,10 +1550,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1569,10 +1561,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1580,10 +1572,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -1591,10 +1583,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -1602,10 +1594,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -1613,10 +1605,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1624,10 +1616,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1635,10 +1627,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1649,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1660,7 +1652,7 @@
         <v>23</v>
       </c>
       <c r="B83" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1671,7 +1663,7 @@
         <v>23</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1682,7 +1674,7 @@
         <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -1693,7 +1685,7 @@
         <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -1704,7 +1696,7 @@
         <v>24</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -1715,7 +1707,7 @@
         <v>24</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -1726,7 +1718,7 @@
         <v>24</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -1737,7 +1729,7 @@
         <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -1748,7 +1740,7 @@
         <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -1759,7 +1751,7 @@
         <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -1770,7 +1762,7 @@
         <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -1781,7 +1773,7 @@
         <v>26</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -1792,7 +1784,7 @@
         <v>26</v>
       </c>
       <c r="B95" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -1803,7 +1795,7 @@
         <v>26</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -1814,7 +1806,7 @@
         <v>26</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -1825,7 +1817,7 @@
         <v>27</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -1836,7 +1828,7 @@
         <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -1847,7 +1839,7 @@
         <v>27</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -1858,7 +1850,7 @@
         <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -1869,7 +1861,7 @@
         <v>28</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -1880,7 +1872,7 @@
         <v>28</v>
       </c>
       <c r="B103" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -1891,7 +1883,7 @@
         <v>28</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -1902,7 +1894,7 @@
         <v>28</v>
       </c>
       <c r="B105" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -1913,7 +1905,7 @@
         <v>29</v>
       </c>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -1924,7 +1916,7 @@
         <v>29</v>
       </c>
       <c r="B107" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -1935,7 +1927,7 @@
         <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -1946,7 +1938,7 @@
         <v>29</v>
       </c>
       <c r="B109" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -1957,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="B110" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -1968,7 +1960,7 @@
         <v>30</v>
       </c>
       <c r="B111" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -1979,7 +1971,7 @@
         <v>30</v>
       </c>
       <c r="B112" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -1990,7 +1982,7 @@
         <v>30</v>
       </c>
       <c r="B113" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2001,7 +1993,7 @@
         <v>31</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2012,7 +2004,7 @@
         <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2023,7 +2015,7 @@
         <v>31</v>
       </c>
       <c r="B116" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2034,7 +2026,7 @@
         <v>31</v>
       </c>
       <c r="B117" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -2045,7 +2037,7 @@
         <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -2056,7 +2048,7 @@
         <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -2067,7 +2059,7 @@
         <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -2078,7 +2070,7 @@
         <v>32</v>
       </c>
       <c r="B121" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -2089,7 +2081,7 @@
         <v>33</v>
       </c>
       <c r="B122" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -2100,7 +2092,7 @@
         <v>33</v>
       </c>
       <c r="B123" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -2111,7 +2103,7 @@
         <v>33</v>
       </c>
       <c r="B124" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -2122,7 +2114,7 @@
         <v>33</v>
       </c>
       <c r="B125" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -2133,7 +2125,7 @@
         <v>34</v>
       </c>
       <c r="B126" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -2144,7 +2136,7 @@
         <v>34</v>
       </c>
       <c r="B127" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -2155,7 +2147,7 @@
         <v>34</v>
       </c>
       <c r="B128" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -2166,7 +2158,7 @@
         <v>34</v>
       </c>
       <c r="B129" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -2177,7 +2169,7 @@
         <v>35</v>
       </c>
       <c r="B130" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2188,7 +2180,7 @@
         <v>35</v>
       </c>
       <c r="B131" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2199,7 +2191,7 @@
         <v>35</v>
       </c>
       <c r="B132" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2210,7 +2202,7 @@
         <v>35</v>
       </c>
       <c r="B133" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2221,7 +2213,7 @@
         <v>36</v>
       </c>
       <c r="B134" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2232,7 +2224,7 @@
         <v>36</v>
       </c>
       <c r="B135" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2243,7 +2235,7 @@
         <v>36</v>
       </c>
       <c r="B136" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2254,7 +2246,7 @@
         <v>36</v>
       </c>
       <c r="B137" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2265,7 +2257,7 @@
         <v>37</v>
       </c>
       <c r="B138" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2276,7 +2268,7 @@
         <v>37</v>
       </c>
       <c r="B139" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2287,7 +2279,7 @@
         <v>37</v>
       </c>
       <c r="B140" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2298,7 +2290,7 @@
         <v>37</v>
       </c>
       <c r="B141" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -2309,7 +2301,7 @@
         <v>38</v>
       </c>
       <c r="B142" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -2320,7 +2312,7 @@
         <v>38</v>
       </c>
       <c r="B143" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -2331,7 +2323,7 @@
         <v>38</v>
       </c>
       <c r="B144" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -2342,7 +2334,7 @@
         <v>38</v>
       </c>
       <c r="B145" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -2353,7 +2345,7 @@
         <v>39</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -2364,7 +2356,7 @@
         <v>39</v>
       </c>
       <c r="B147" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -2375,7 +2367,7 @@
         <v>39</v>
       </c>
       <c r="B148" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -2386,7 +2378,7 @@
         <v>39</v>
       </c>
       <c r="B149" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -2397,7 +2389,7 @@
         <v>40</v>
       </c>
       <c r="B150" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -2408,7 +2400,7 @@
         <v>40</v>
       </c>
       <c r="B151" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -2419,7 +2411,7 @@
         <v>40</v>
       </c>
       <c r="B152" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -2430,7 +2422,7 @@
         <v>40</v>
       </c>
       <c r="B153" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -2441,7 +2433,7 @@
         <v>41</v>
       </c>
       <c r="B154" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -2452,7 +2444,7 @@
         <v>41</v>
       </c>
       <c r="B155" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -2463,7 +2455,7 @@
         <v>41</v>
       </c>
       <c r="B156" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -2474,7 +2466,7 @@
         <v>41</v>
       </c>
       <c r="B157" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -2485,7 +2477,7 @@
         <v>42</v>
       </c>
       <c r="B158" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -2496,7 +2488,7 @@
         <v>42</v>
       </c>
       <c r="B159" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -2507,7 +2499,7 @@
         <v>42</v>
       </c>
       <c r="B160" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -2518,7 +2510,7 @@
         <v>42</v>
       </c>
       <c r="B161" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -2529,7 +2521,7 @@
         <v>43</v>
       </c>
       <c r="B162" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -2540,7 +2532,7 @@
         <v>43</v>
       </c>
       <c r="B163" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -2551,7 +2543,7 @@
         <v>43</v>
       </c>
       <c r="B164" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -2562,7 +2554,7 @@
         <v>43</v>
       </c>
       <c r="B165" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -2573,7 +2565,7 @@
         <v>44</v>
       </c>
       <c r="B166" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -2584,7 +2576,7 @@
         <v>44</v>
       </c>
       <c r="B167" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -2595,7 +2587,7 @@
         <v>44</v>
       </c>
       <c r="B168" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -2606,7 +2598,7 @@
         <v>44</v>
       </c>
       <c r="B169" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C169">
         <v>0</v>
@@ -2617,7 +2609,7 @@
         <v>45</v>
       </c>
       <c r="B170" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -2628,7 +2620,7 @@
         <v>45</v>
       </c>
       <c r="B171" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -2639,7 +2631,7 @@
         <v>45</v>
       </c>
       <c r="B172" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -2650,7 +2642,7 @@
         <v>45</v>
       </c>
       <c r="B173" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -2661,7 +2653,7 @@
         <v>46</v>
       </c>
       <c r="B174" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -2672,7 +2664,7 @@
         <v>46</v>
       </c>
       <c r="B175" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -2683,7 +2675,7 @@
         <v>46</v>
       </c>
       <c r="B176" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -2694,7 +2686,7 @@
         <v>46</v>
       </c>
       <c r="B177" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -2705,7 +2697,7 @@
         <v>47</v>
       </c>
       <c r="B178" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C178">
         <v>0</v>
@@ -2716,7 +2708,7 @@
         <v>47</v>
       </c>
       <c r="B179" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -2727,7 +2719,7 @@
         <v>47</v>
       </c>
       <c r="B180" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -2738,7 +2730,7 @@
         <v>47</v>
       </c>
       <c r="B181" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -2749,7 +2741,7 @@
         <v>48</v>
       </c>
       <c r="B182" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -2760,7 +2752,7 @@
         <v>48</v>
       </c>
       <c r="B183" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -2771,7 +2763,7 @@
         <v>48</v>
       </c>
       <c r="B184" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -2782,7 +2774,7 @@
         <v>48</v>
       </c>
       <c r="B185" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -2793,7 +2785,7 @@
         <v>49</v>
       </c>
       <c r="B186" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C186">
         <v>0</v>
@@ -2804,7 +2796,7 @@
         <v>49</v>
       </c>
       <c r="B187" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -2815,7 +2807,7 @@
         <v>49</v>
       </c>
       <c r="B188" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C188">
         <v>0</v>
@@ -2826,7 +2818,7 @@
         <v>49</v>
       </c>
       <c r="B189" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -2837,7 +2829,7 @@
         <v>50</v>
       </c>
       <c r="B190" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -2848,7 +2840,7 @@
         <v>50</v>
       </c>
       <c r="B191" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -2859,7 +2851,7 @@
         <v>50</v>
       </c>
       <c r="B192" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -2870,7 +2862,7 @@
         <v>50</v>
       </c>
       <c r="B193" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C193">
         <v>0</v>
@@ -2881,7 +2873,7 @@
         <v>51</v>
       </c>
       <c r="B194" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C194">
         <v>0</v>
@@ -2892,7 +2884,7 @@
         <v>51</v>
       </c>
       <c r="B195" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C195">
         <v>0</v>
@@ -2903,7 +2895,7 @@
         <v>51</v>
       </c>
       <c r="B196" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C196">
         <v>0</v>
@@ -2914,7 +2906,7 @@
         <v>51</v>
       </c>
       <c r="B197" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C197">
         <v>0</v>
@@ -2925,7 +2917,7 @@
         <v>52</v>
       </c>
       <c r="B198" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C198">
         <v>0</v>
@@ -2936,7 +2928,7 @@
         <v>52</v>
       </c>
       <c r="B199" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C199">
         <v>0</v>
@@ -2947,7 +2939,7 @@
         <v>52</v>
       </c>
       <c r="B200" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C200">
         <v>0</v>
@@ -2958,7 +2950,7 @@
         <v>52</v>
       </c>
       <c r="B201" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C201">
         <v>0</v>
@@ -2969,7 +2961,7 @@
         <v>53</v>
       </c>
       <c r="B202" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C202">
         <v>0</v>
@@ -2980,7 +2972,7 @@
         <v>53</v>
       </c>
       <c r="B203" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C203">
         <v>0</v>
@@ -2991,7 +2983,7 @@
         <v>53</v>
       </c>
       <c r="B204" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C204">
         <v>0</v>
@@ -3002,7 +2994,7 @@
         <v>53</v>
       </c>
       <c r="B205" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C205">
         <v>0</v>
@@ -3013,7 +3005,7 @@
         <v>54</v>
       </c>
       <c r="B206" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C206">
         <v>0</v>
@@ -3024,7 +3016,7 @@
         <v>54</v>
       </c>
       <c r="B207" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C207">
         <v>0</v>
@@ -3035,7 +3027,7 @@
         <v>54</v>
       </c>
       <c r="B208" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C208">
         <v>0</v>
@@ -3046,7 +3038,7 @@
         <v>54</v>
       </c>
       <c r="B209" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C209">
         <v>0</v>
@@ -3057,7 +3049,7 @@
         <v>55</v>
       </c>
       <c r="B210" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C210">
         <v>0</v>
@@ -3068,7 +3060,7 @@
         <v>55</v>
       </c>
       <c r="B211" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C211">
         <v>0</v>
@@ -3079,7 +3071,7 @@
         <v>55</v>
       </c>
       <c r="B212" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C212">
         <v>0</v>
@@ -3090,7 +3082,7 @@
         <v>55</v>
       </c>
       <c r="B213" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C213">
         <v>0</v>
@@ -3101,7 +3093,7 @@
         <v>56</v>
       </c>
       <c r="B214" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C214">
         <v>0</v>
@@ -3112,7 +3104,7 @@
         <v>56</v>
       </c>
       <c r="B215" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C215">
         <v>0</v>
@@ -3123,7 +3115,7 @@
         <v>56</v>
       </c>
       <c r="B216" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C216">
         <v>0</v>
@@ -3134,7 +3126,7 @@
         <v>56</v>
       </c>
       <c r="B217" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C217">
         <v>0</v>
@@ -3145,7 +3137,7 @@
         <v>57</v>
       </c>
       <c r="B218" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C218">
         <v>0</v>
@@ -3156,7 +3148,7 @@
         <v>57</v>
       </c>
       <c r="B219" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C219">
         <v>0</v>
@@ -3167,7 +3159,7 @@
         <v>57</v>
       </c>
       <c r="B220" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C220">
         <v>0</v>
@@ -3178,7 +3170,7 @@
         <v>57</v>
       </c>
       <c r="B221" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C221">
         <v>0</v>
@@ -3189,7 +3181,7 @@
         <v>58</v>
       </c>
       <c r="B222" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C222">
         <v>0</v>
@@ -3200,7 +3192,7 @@
         <v>58</v>
       </c>
       <c r="B223" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C223">
         <v>0</v>
@@ -3211,7 +3203,7 @@
         <v>58</v>
       </c>
       <c r="B224" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C224">
         <v>0</v>
@@ -3222,7 +3214,7 @@
         <v>58</v>
       </c>
       <c r="B225" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C225">
         <v>0</v>
@@ -3233,7 +3225,7 @@
         <v>59</v>
       </c>
       <c r="B226" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C226">
         <v>0</v>
@@ -3244,7 +3236,7 @@
         <v>59</v>
       </c>
       <c r="B227" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C227">
         <v>0</v>
@@ -3255,7 +3247,7 @@
         <v>59</v>
       </c>
       <c r="B228" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C228">
         <v>0</v>
@@ -3266,7 +3258,7 @@
         <v>59</v>
       </c>
       <c r="B229" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C229">
         <v>0</v>
@@ -3277,7 +3269,7 @@
         <v>60</v>
       </c>
       <c r="B230" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C230">
         <v>0</v>
@@ -3288,7 +3280,7 @@
         <v>60</v>
       </c>
       <c r="B231" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C231">
         <v>0</v>
@@ -3299,7 +3291,7 @@
         <v>60</v>
       </c>
       <c r="B232" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C232">
         <v>0</v>
@@ -3310,7 +3302,7 @@
         <v>60</v>
       </c>
       <c r="B233" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C233">
         <v>0</v>
@@ -3321,7 +3313,7 @@
         <v>61</v>
       </c>
       <c r="B234" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C234">
         <v>0</v>
@@ -3332,7 +3324,7 @@
         <v>61</v>
       </c>
       <c r="B235" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C235">
         <v>0</v>
@@ -3343,7 +3335,7 @@
         <v>61</v>
       </c>
       <c r="B236" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C236">
         <v>0</v>
@@ -3354,7 +3346,7 @@
         <v>61</v>
       </c>
       <c r="B237" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C237">
         <v>0</v>
@@ -3365,7 +3357,7 @@
         <v>62</v>
       </c>
       <c r="B238" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C238">
         <v>0</v>
@@ -3376,7 +3368,7 @@
         <v>62</v>
       </c>
       <c r="B239" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C239">
         <v>0</v>
@@ -3387,7 +3379,7 @@
         <v>62</v>
       </c>
       <c r="B240" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C240">
         <v>0</v>
@@ -3398,7 +3390,7 @@
         <v>62</v>
       </c>
       <c r="B241" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C241">
         <v>0</v>
@@ -3409,7 +3401,7 @@
         <v>63</v>
       </c>
       <c r="B242" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C242">
         <v>0</v>
@@ -3420,7 +3412,7 @@
         <v>63</v>
       </c>
       <c r="B243" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C243">
         <v>0</v>
@@ -3431,7 +3423,7 @@
         <v>63</v>
       </c>
       <c r="B244" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C244">
         <v>0</v>
@@ -3442,7 +3434,7 @@
         <v>63</v>
       </c>
       <c r="B245" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C245">
         <v>0</v>
@@ -3453,7 +3445,7 @@
         <v>64</v>
       </c>
       <c r="B246" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C246">
         <v>0</v>
@@ -3464,7 +3456,7 @@
         <v>64</v>
       </c>
       <c r="B247" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C247">
         <v>0</v>
@@ -3475,7 +3467,7 @@
         <v>64</v>
       </c>
       <c r="B248" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C248">
         <v>0</v>
@@ -3486,7 +3478,7 @@
         <v>64</v>
       </c>
       <c r="B249" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C249">
         <v>0</v>
@@ -3497,7 +3489,7 @@
         <v>65</v>
       </c>
       <c r="B250" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C250">
         <v>0</v>
@@ -3508,7 +3500,7 @@
         <v>65</v>
       </c>
       <c r="B251" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C251">
         <v>0</v>
@@ -3519,7 +3511,7 @@
         <v>65</v>
       </c>
       <c r="B252" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C252">
         <v>0</v>
@@ -3530,7 +3522,7 @@
         <v>65</v>
       </c>
       <c r="B253" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C253">
         <v>0</v>
@@ -3541,7 +3533,7 @@
         <v>66</v>
       </c>
       <c r="B254" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C254">
         <v>0</v>
@@ -3552,7 +3544,7 @@
         <v>66</v>
       </c>
       <c r="B255" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C255">
         <v>0</v>
@@ -3563,7 +3555,7 @@
         <v>66</v>
       </c>
       <c r="B256" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C256">
         <v>0</v>
@@ -3574,7 +3566,7 @@
         <v>66</v>
       </c>
       <c r="B257" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C257">
         <v>0</v>
@@ -3585,7 +3577,7 @@
         <v>67</v>
       </c>
       <c r="B258" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C258">
         <v>0</v>
@@ -3596,7 +3588,7 @@
         <v>67</v>
       </c>
       <c r="B259" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C259">
         <v>0</v>
@@ -3607,7 +3599,7 @@
         <v>67</v>
       </c>
       <c r="B260" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C260">
         <v>0</v>
@@ -3618,7 +3610,7 @@
         <v>67</v>
       </c>
       <c r="B261" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C261">
         <v>0</v>
@@ -3629,7 +3621,7 @@
         <v>68</v>
       </c>
       <c r="B262" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C262">
         <v>0</v>
@@ -3640,7 +3632,7 @@
         <v>68</v>
       </c>
       <c r="B263" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C263">
         <v>0</v>
@@ -3651,7 +3643,7 @@
         <v>68</v>
       </c>
       <c r="B264" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C264">
         <v>0</v>
@@ -3662,7 +3654,7 @@
         <v>68</v>
       </c>
       <c r="B265" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C265">
         <v>0</v>
@@ -3673,7 +3665,7 @@
         <v>69</v>
       </c>
       <c r="B266" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C266">
         <v>0</v>
@@ -3684,7 +3676,7 @@
         <v>69</v>
       </c>
       <c r="B267" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C267">
         <v>0</v>
@@ -3695,7 +3687,7 @@
         <v>69</v>
       </c>
       <c r="B268" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C268">
         <v>0</v>
@@ -3706,7 +3698,7 @@
         <v>69</v>
       </c>
       <c r="B269" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C269">
         <v>0</v>
@@ -3717,7 +3709,7 @@
         <v>70</v>
       </c>
       <c r="B270" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C270">
         <v>0</v>
@@ -3728,7 +3720,7 @@
         <v>70</v>
       </c>
       <c r="B271" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C271">
         <v>0</v>
@@ -3739,7 +3731,7 @@
         <v>70</v>
       </c>
       <c r="B272" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C272">
         <v>0</v>
@@ -3750,7 +3742,7 @@
         <v>70</v>
       </c>
       <c r="B273" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C273">
         <v>0</v>
@@ -3761,7 +3753,7 @@
         <v>71</v>
       </c>
       <c r="B274" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C274">
         <v>0</v>
@@ -3772,7 +3764,7 @@
         <v>71</v>
       </c>
       <c r="B275" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C275">
         <v>0</v>
@@ -3783,7 +3775,7 @@
         <v>71</v>
       </c>
       <c r="B276" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C276">
         <v>0</v>
@@ -3794,7 +3786,7 @@
         <v>71</v>
       </c>
       <c r="B277" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C277">
         <v>0</v>
@@ -3805,7 +3797,7 @@
         <v>72</v>
       </c>
       <c r="B278" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C278">
         <v>0</v>
@@ -3816,7 +3808,7 @@
         <v>72</v>
       </c>
       <c r="B279" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C279">
         <v>0</v>
@@ -3827,7 +3819,7 @@
         <v>72</v>
       </c>
       <c r="B280" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C280">
         <v>0</v>
@@ -3838,7 +3830,7 @@
         <v>72</v>
       </c>
       <c r="B281" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C281">
         <v>0</v>
@@ -3849,7 +3841,7 @@
         <v>73</v>
       </c>
       <c r="B282" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C282">
         <v>0</v>
@@ -3860,7 +3852,7 @@
         <v>73</v>
       </c>
       <c r="B283" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C283">
         <v>0</v>
@@ -3871,7 +3863,7 @@
         <v>73</v>
       </c>
       <c r="B284" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -3882,7 +3874,7 @@
         <v>73</v>
       </c>
       <c r="B285" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C285">
         <v>0</v>
@@ -3893,7 +3885,7 @@
         <v>74</v>
       </c>
       <c r="B286" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C286">
         <v>0</v>
@@ -3904,7 +3896,7 @@
         <v>74</v>
       </c>
       <c r="B287" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C287">
         <v>0</v>
@@ -3915,7 +3907,7 @@
         <v>74</v>
       </c>
       <c r="B288" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C288">
         <v>0</v>
@@ -3926,7 +3918,7 @@
         <v>74</v>
       </c>
       <c r="B289" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C289">
         <v>0</v>
@@ -3937,7 +3929,7 @@
         <v>75</v>
       </c>
       <c r="B290" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C290">
         <v>0</v>
@@ -3948,7 +3940,7 @@
         <v>75</v>
       </c>
       <c r="B291" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C291">
         <v>0</v>
@@ -3959,7 +3951,7 @@
         <v>75</v>
       </c>
       <c r="B292" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C292">
         <v>0</v>
@@ -3970,7 +3962,7 @@
         <v>75</v>
       </c>
       <c r="B293" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C293">
         <v>0</v>
@@ -3981,7 +3973,7 @@
         <v>76</v>
       </c>
       <c r="B294" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C294">
         <v>0</v>
@@ -3992,7 +3984,7 @@
         <v>76</v>
       </c>
       <c r="B295" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C295">
         <v>0</v>
@@ -4003,7 +3995,7 @@
         <v>76</v>
       </c>
       <c r="B296" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C296">
         <v>0</v>
@@ -4014,7 +4006,7 @@
         <v>76</v>
       </c>
       <c r="B297" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C297">
         <v>0</v>
@@ -4025,7 +4017,7 @@
         <v>77</v>
       </c>
       <c r="B298" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C298">
         <v>0</v>
@@ -4036,7 +4028,7 @@
         <v>77</v>
       </c>
       <c r="B299" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C299">
         <v>0</v>
@@ -4047,7 +4039,7 @@
         <v>77</v>
       </c>
       <c r="B300" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C300">
         <v>0</v>
@@ -4058,7 +4050,7 @@
         <v>77</v>
       </c>
       <c r="B301" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C301">
         <v>0</v>
@@ -4069,7 +4061,7 @@
         <v>78</v>
       </c>
       <c r="B302" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C302">
         <v>0</v>
@@ -4080,7 +4072,7 @@
         <v>78</v>
       </c>
       <c r="B303" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C303">
         <v>0</v>
@@ -4091,7 +4083,7 @@
         <v>78</v>
       </c>
       <c r="B304" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C304">
         <v>0</v>
@@ -4102,7 +4094,7 @@
         <v>78</v>
       </c>
       <c r="B305" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C305">
         <v>0</v>
@@ -4113,7 +4105,7 @@
         <v>79</v>
       </c>
       <c r="B306" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C306">
         <v>0</v>
@@ -4124,7 +4116,7 @@
         <v>79</v>
       </c>
       <c r="B307" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C307">
         <v>0</v>
@@ -4135,7 +4127,7 @@
         <v>79</v>
       </c>
       <c r="B308" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C308">
         <v>0</v>
@@ -4146,7 +4138,7 @@
         <v>79</v>
       </c>
       <c r="B309" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C309">
         <v>0</v>
@@ -4157,7 +4149,7 @@
         <v>80</v>
       </c>
       <c r="B310" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C310">
         <v>0</v>
@@ -4168,7 +4160,7 @@
         <v>80</v>
       </c>
       <c r="B311" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C311">
         <v>0</v>
@@ -4179,7 +4171,7 @@
         <v>80</v>
       </c>
       <c r="B312" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C312">
         <v>0</v>
@@ -4190,7 +4182,7 @@
         <v>80</v>
       </c>
       <c r="B313" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C313">
         <v>0</v>
@@ -4201,7 +4193,7 @@
         <v>81</v>
       </c>
       <c r="B314" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C314">
         <v>0</v>
@@ -4212,7 +4204,7 @@
         <v>81</v>
       </c>
       <c r="B315" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C315">
         <v>0</v>
@@ -4223,7 +4215,7 @@
         <v>81</v>
       </c>
       <c r="B316" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C316">
         <v>0</v>
@@ -4234,7 +4226,7 @@
         <v>81</v>
       </c>
       <c r="B317" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C317">
         <v>0</v>
@@ -4245,7 +4237,7 @@
         <v>82</v>
       </c>
       <c r="B318" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C318">
         <v>0</v>
@@ -4256,7 +4248,7 @@
         <v>82</v>
       </c>
       <c r="B319" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C319">
         <v>0</v>
@@ -4267,7 +4259,7 @@
         <v>82</v>
       </c>
       <c r="B320" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C320">
         <v>0</v>
@@ -4278,7 +4270,7 @@
         <v>82</v>
       </c>
       <c r="B321" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C321">
         <v>0</v>
@@ -4289,7 +4281,7 @@
         <v>83</v>
       </c>
       <c r="B322" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C322">
         <v>0</v>
@@ -4300,7 +4292,7 @@
         <v>83</v>
       </c>
       <c r="B323" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C323">
         <v>0</v>
@@ -4311,7 +4303,7 @@
         <v>83</v>
       </c>
       <c r="B324" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C324">
         <v>0</v>
@@ -4322,7 +4314,7 @@
         <v>83</v>
       </c>
       <c r="B325" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C325">
         <v>0</v>
@@ -4333,7 +4325,7 @@
         <v>84</v>
       </c>
       <c r="B326" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C326">
         <v>0</v>
@@ -4344,7 +4336,7 @@
         <v>84</v>
       </c>
       <c r="B327" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C327">
         <v>0</v>
@@ -4355,7 +4347,7 @@
         <v>84</v>
       </c>
       <c r="B328" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C328">
         <v>0</v>
@@ -4366,7 +4358,7 @@
         <v>84</v>
       </c>
       <c r="B329" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C329">
         <v>0</v>
@@ -4377,7 +4369,7 @@
         <v>85</v>
       </c>
       <c r="B330" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C330">
         <v>0</v>
@@ -4388,7 +4380,7 @@
         <v>85</v>
       </c>
       <c r="B331" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C331">
         <v>0</v>
@@ -4399,7 +4391,7 @@
         <v>85</v>
       </c>
       <c r="B332" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C332">
         <v>0</v>
@@ -4410,7 +4402,7 @@
         <v>85</v>
       </c>
       <c r="B333" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C333">
         <v>0</v>
@@ -4421,7 +4413,7 @@
         <v>86</v>
       </c>
       <c r="B334" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C334">
         <v>0</v>
@@ -4432,7 +4424,7 @@
         <v>86</v>
       </c>
       <c r="B335" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C335">
         <v>0</v>
@@ -4443,7 +4435,7 @@
         <v>86</v>
       </c>
       <c r="B336" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C336">
         <v>0</v>
@@ -4454,7 +4446,7 @@
         <v>86</v>
       </c>
       <c r="B337" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C337">
         <v>0</v>
@@ -4465,7 +4457,7 @@
         <v>87</v>
       </c>
       <c r="B338" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C338">
         <v>0</v>
@@ -4476,7 +4468,7 @@
         <v>87</v>
       </c>
       <c r="B339" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C339">
         <v>0</v>
@@ -4487,7 +4479,7 @@
         <v>87</v>
       </c>
       <c r="B340" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C340">
         <v>0</v>
@@ -4498,7 +4490,7 @@
         <v>87</v>
       </c>
       <c r="B341" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C341">
         <v>0</v>
@@ -4509,7 +4501,7 @@
         <v>88</v>
       </c>
       <c r="B342" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C342">
         <v>0</v>
@@ -4520,7 +4512,7 @@
         <v>88</v>
       </c>
       <c r="B343" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C343">
         <v>0</v>
@@ -4531,7 +4523,7 @@
         <v>88</v>
       </c>
       <c r="B344" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C344">
         <v>0</v>
@@ -4542,7 +4534,7 @@
         <v>88</v>
       </c>
       <c r="B345" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C345">
         <v>0</v>
@@ -4553,7 +4545,7 @@
         <v>89</v>
       </c>
       <c r="B346" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C346">
         <v>0</v>
@@ -4564,7 +4556,7 @@
         <v>89</v>
       </c>
       <c r="B347" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C347">
         <v>0</v>
@@ -4575,7 +4567,7 @@
         <v>89</v>
       </c>
       <c r="B348" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C348">
         <v>0</v>
@@ -4586,7 +4578,7 @@
         <v>89</v>
       </c>
       <c r="B349" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C349">
         <v>0</v>
@@ -4597,7 +4589,7 @@
         <v>90</v>
       </c>
       <c r="B350" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C350">
         <v>0</v>
@@ -4608,7 +4600,7 @@
         <v>90</v>
       </c>
       <c r="B351" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C351">
         <v>0</v>
@@ -4619,7 +4611,7 @@
         <v>90</v>
       </c>
       <c r="B352" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C352">
         <v>0</v>
@@ -4630,7 +4622,7 @@
         <v>90</v>
       </c>
       <c r="B353" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C353">
         <v>0</v>
@@ -4641,7 +4633,7 @@
         <v>91</v>
       </c>
       <c r="B354" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C354">
         <v>0</v>
@@ -4652,7 +4644,7 @@
         <v>91</v>
       </c>
       <c r="B355" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C355">
         <v>0</v>
@@ -4663,7 +4655,7 @@
         <v>91</v>
       </c>
       <c r="B356" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C356">
         <v>0</v>
@@ -4674,7 +4666,7 @@
         <v>91</v>
       </c>
       <c r="B357" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C357">
         <v>0</v>
@@ -4685,7 +4677,7 @@
         <v>92</v>
       </c>
       <c r="B358" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C358">
         <v>0</v>
@@ -4696,7 +4688,7 @@
         <v>92</v>
       </c>
       <c r="B359" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C359">
         <v>0</v>
@@ -4707,7 +4699,7 @@
         <v>92</v>
       </c>
       <c r="B360" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C360">
         <v>0</v>
@@ -4718,7 +4710,7 @@
         <v>92</v>
       </c>
       <c r="B361" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C361">
         <v>0</v>
@@ -4729,7 +4721,7 @@
         <v>93</v>
       </c>
       <c r="B362" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C362">
         <v>0</v>
@@ -4740,7 +4732,7 @@
         <v>93</v>
       </c>
       <c r="B363" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C363">
         <v>0</v>
@@ -4751,7 +4743,7 @@
         <v>93</v>
       </c>
       <c r="B364" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C364">
         <v>0</v>
@@ -4762,7 +4754,7 @@
         <v>93</v>
       </c>
       <c r="B365" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C365">
         <v>0</v>
@@ -4773,7 +4765,7 @@
         <v>94</v>
       </c>
       <c r="B366" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C366">
         <v>0</v>
@@ -4784,7 +4776,7 @@
         <v>94</v>
       </c>
       <c r="B367" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C367">
         <v>0</v>
@@ -4795,7 +4787,7 @@
         <v>94</v>
       </c>
       <c r="B368" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C368">
         <v>0</v>
@@ -4806,7 +4798,7 @@
         <v>94</v>
       </c>
       <c r="B369" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C369">
         <v>0</v>
@@ -4817,7 +4809,7 @@
         <v>95</v>
       </c>
       <c r="B370" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C370">
         <v>0</v>
@@ -4828,7 +4820,7 @@
         <v>95</v>
       </c>
       <c r="B371" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C371">
         <v>0</v>
@@ -4839,7 +4831,7 @@
         <v>95</v>
       </c>
       <c r="B372" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C372">
         <v>0</v>
@@ -4850,7 +4842,7 @@
         <v>95</v>
       </c>
       <c r="B373" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C373">
         <v>0</v>
@@ -4861,7 +4853,7 @@
         <v>96</v>
       </c>
       <c r="B374" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C374">
         <v>0</v>
@@ -4872,7 +4864,7 @@
         <v>96</v>
       </c>
       <c r="B375" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C375">
         <v>0</v>
@@ -4883,7 +4875,7 @@
         <v>96</v>
       </c>
       <c r="B376" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C376">
         <v>0</v>
@@ -4894,97 +4886,9 @@
         <v>96</v>
       </c>
       <c r="B377" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C377">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A378" t="s">
-        <v>97</v>
-      </c>
-      <c r="B378" t="s">
-        <v>99</v>
-      </c>
-      <c r="C378">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A379" t="s">
-        <v>97</v>
-      </c>
-      <c r="B379" t="s">
-        <v>100</v>
-      </c>
-      <c r="C379">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A380" t="s">
-        <v>97</v>
-      </c>
-      <c r="B380" t="s">
-        <v>102</v>
-      </c>
-      <c r="C380">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A381" t="s">
-        <v>97</v>
-      </c>
-      <c r="B381" t="s">
-        <v>101</v>
-      </c>
-      <c r="C381">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A382" t="s">
-        <v>98</v>
-      </c>
-      <c r="B382" t="s">
-        <v>99</v>
-      </c>
-      <c r="C382">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A383" t="s">
-        <v>98</v>
-      </c>
-      <c r="B383" t="s">
-        <v>100</v>
-      </c>
-      <c r="C383">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A384" t="s">
-        <v>98</v>
-      </c>
-      <c r="B384" t="s">
-        <v>102</v>
-      </c>
-      <c r="C384">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A385" t="s">
-        <v>98</v>
-      </c>
-      <c r="B385" t="s">
-        <v>101</v>
-      </c>
-      <c r="C385">
         <v>0</v>
       </c>
     </row>

</xml_diff>